<commit_message>
add KartaOcenyProjektu_1.xlsx & update other documents
</commit_message>
<xml_diff>
--- a/documents & instructions/inflation.xlsx
+++ b/documents & instructions/inflation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\source\finance-and-investing\documents &amp; instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE506C2-CE94-4EB0-B76F-7DD3D29880AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40B7C49-A84B-4F24-9657-0031D25E8B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <t>Inflation</t>
   </si>
   <si>
-    <t>Cumulative inflation</t>
+    <t>CumulativeInflation</t>
   </si>
 </sst>
 </file>
@@ -55,8 +55,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;zł&quot;"/>
-    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -90,8 +90,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -551,7 +551,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cumulative inflation</c:v>
+                  <c:v>CumulativeInflation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -644,64 +644,64 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.179</c:v>
+                  <c:v>0.17900000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3900410000000001</c:v>
+                  <c:v>0.39004100000000008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6388583390000002</c:v>
+                  <c:v>0.63885833900000022</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9322139816810004</c:v>
+                  <c:v>0.93221398168100045</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2780802844018995</c:v>
+                  <c:v>1.2780802844018995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.6858566553098395</c:v>
+                  <c:v>1.6858566553098395</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1666249966103011</c:v>
+                  <c:v>2.1666249966103011</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.7334508710035452</c:v>
+                  <c:v>2.7334508710035452</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.4017385769131803</c:v>
+                  <c:v>3.4017385769131803</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.1896497821806395</c:v>
+                  <c:v>4.1896497821806395</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.1185970931909743</c:v>
+                  <c:v>5.1185970931909743</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.2138259728721588</c:v>
+                  <c:v>6.2138259728721588</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.505100822016276</c:v>
+                  <c:v>7.505100822016276</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10.02751386915719</c:v>
+                  <c:v>9.0275138691571897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.822438851736328</c:v>
+                  <c:v>10.822438851736328</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13.938655406197132</c:v>
+                  <c:v>12.938655406197132</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16.433674723906417</c:v>
+                  <c:v>15.433674723906417</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.375302499485667</c:v>
+                  <c:v>18.375302499485667</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>22.843481646893601</c:v>
+                  <c:v>21.843481646893601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -887,6 +887,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="638765448"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1817,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1856,7 +1857,7 @@
         <v>0.17899999999999999</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
         <f>(B21-B2)/B2</f>
@@ -1885,8 +1886,8 @@
         <v>0.17899999999999999</v>
       </c>
       <c r="D3" s="1">
-        <f>D2*(1+C2)</f>
-        <v>1.179</v>
+        <f>(D2+1)*(C2+1)-1</f>
+        <v>0.17900000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1901,8 +1902,8 @@
         <v>0.17899999999999999</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D21" si="1">D3*(1+C3)</f>
-        <v>1.3900410000000001</v>
+        <f t="shared" ref="D4:D21" si="1">(D3+1)*(C3+1)-1</f>
+        <v>0.39004100000000008</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1918,7 +1919,7 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>1.6388583390000002</v>
+        <v>0.63885833900000022</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1934,7 +1935,7 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>1.9322139816810004</v>
+        <v>0.93221398168100045</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1950,7 +1951,7 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>2.2780802844018995</v>
+        <v>1.2780802844018995</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1966,7 +1967,7 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>2.6858566553098395</v>
+        <v>1.6858566553098395</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1982,7 +1983,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>3.1666249966103011</v>
+        <v>2.1666249966103011</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1998,7 +1999,7 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>3.7334508710035452</v>
+        <v>2.7334508710035452</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -2014,7 +2015,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>4.4017385769131803</v>
+        <v>3.4017385769131803</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -2030,7 +2031,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>5.1896497821806395</v>
+        <v>4.1896497821806395</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -2046,7 +2047,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>6.1185970931909743</v>
+        <v>5.1185970931909743</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -2062,7 +2063,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>7.2138259728721588</v>
+        <v>6.2138259728721588</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -2078,7 +2079,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>8.505100822016276</v>
+        <v>7.505100822016276</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -2094,7 +2095,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>10.02751386915719</v>
+        <v>9.0275138691571897</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -2110,7 +2111,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>11.822438851736328</v>
+        <v>10.822438851736328</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -2126,7 +2127,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>13.938655406197132</v>
+        <v>12.938655406197132</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -2142,7 +2143,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" si="1"/>
-        <v>16.433674723906417</v>
+        <v>15.433674723906417</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -2158,7 +2159,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" si="1"/>
-        <v>19.375302499485667</v>
+        <v>18.375302499485667</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -2174,7 +2175,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" si="1"/>
-        <v>22.843481646893601</v>
+        <v>21.843481646893601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>